<commit_message>
latest code commited on 15th sept
</commit_message>
<xml_diff>
--- a/Data/CMDB_DataSheet.xlsx
+++ b/Data/CMDB_DataSheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehetrr\git\RemedyTest\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehetrr\git\RemedyTest-1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Alarmkey_Data" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="118">
   <si>
     <t>Description</t>
   </si>
@@ -395,9 +395,6 @@
     <t>Verify_CID</t>
   </si>
   <si>
-    <t>Hardware1</t>
-  </si>
-  <si>
     <t>mnmlw-r730-45.uk.pri.o2.com</t>
   </si>
   <si>
@@ -422,15 +419,9 @@
     <t>Dell1</t>
   </si>
   <si>
-    <t>ambari_agent_version_select1</t>
-  </si>
-  <si>
     <t>ambari_server_agent_heartbeat</t>
   </si>
   <si>
-    <t>Resilience1</t>
-  </si>
-  <si>
     <t>Disaster Recovery Capability</t>
   </si>
   <si>
@@ -479,7 +470,7 @@
     <t>cnmlw-esxvm-222~pam</t>
   </si>
   <si>
-    <t>mnmlw-r730-56_1</t>
+    <t>ambari_agent_version_select</t>
   </si>
 </sst>
 </file>
@@ -674,7 +665,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -803,6 +794,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1204,10 +1198,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1324,8 +1318,8 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
     </row>
     <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1350,7 +1344,7 @@
         <v>3</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>103</v>
+        <v>17</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>18</v>
@@ -1367,15 +1361,15 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
     </row>
     <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="C4" s="6">
         <v>7951</v>
@@ -1410,17 +1404,19 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15"/>
     </row>
     <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="6"/>
+        <v>100</v>
+      </c>
+      <c r="C5" s="6">
+        <v>7951</v>
+      </c>
       <c r="D5" s="3">
         <v>1</v>
       </c>
@@ -1451,8 +1447,20 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D4:J5">
@@ -1511,8 +1519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1694,7 +1702,7 @@
         <v>69</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>92</v>
+        <v>64</v>
       </c>
       <c r="H2" s="26" t="s">
         <v>65</v>
@@ -1779,7 +1787,7 @@
         <v>81</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="F3" s="26" t="s">
         <v>69</v>
@@ -1860,33 +1868,33 @@
       <c r="A4" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="42" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="25" t="s">
-        <v>94</v>
-      </c>
       <c r="D4" s="25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F4" s="27"/>
       <c r="G4" s="26" t="s">
         <v>64</v>
       </c>
       <c r="H4" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I4" s="26" t="s">
         <v>63</v>
       </c>
       <c r="J4" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="K4" s="26" t="s">
         <v>96</v>
-      </c>
-      <c r="K4" s="26" t="s">
-        <v>97</v>
       </c>
       <c r="L4" s="27" t="s">
         <v>66</v>
@@ -1930,38 +1938,44 @@
       <c r="AE4" s="27"/>
       <c r="AF4" s="27"/>
       <c r="AG4" s="27"/>
+      <c r="AH4" s="27"/>
+      <c r="AI4" s="27"/>
+      <c r="AJ4" s="27"/>
+      <c r="AK4" s="27"/>
+      <c r="AL4" s="27"/>
+      <c r="AM4" s="27"/>
     </row>
     <row r="5" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>99</v>
-      </c>
       <c r="D5" s="25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F5" s="27"/>
       <c r="G5" s="26" t="s">
         <v>64</v>
       </c>
       <c r="H5" s="26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I5" s="26" t="s">
         <v>63</v>
       </c>
       <c r="J5" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="K5" s="26" t="s">
         <v>96</v>
-      </c>
-      <c r="K5" s="26" t="s">
-        <v>97</v>
       </c>
       <c r="L5" s="27" t="s">
         <v>66</v>
@@ -2005,6 +2019,12 @@
       <c r="AE5" s="27"/>
       <c r="AF5" s="27"/>
       <c r="AG5" s="27"/>
+      <c r="AH5" s="27"/>
+      <c r="AI5" s="27"/>
+      <c r="AJ5" s="27"/>
+      <c r="AK5" s="27"/>
+      <c r="AL5" s="27"/>
+      <c r="AM5" s="27"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
@@ -2038,7 +2058,7 @@
         <v>70</v>
       </c>
       <c r="K6" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L6" s="26" t="s">
         <v>66</v>
@@ -2088,6 +2108,12 @@
       <c r="AE6" s="27"/>
       <c r="AF6" s="27"/>
       <c r="AG6" s="27"/>
+      <c r="AH6" s="27"/>
+      <c r="AI6" s="27"/>
+      <c r="AJ6" s="27"/>
+      <c r="AK6" s="27"/>
+      <c r="AL6" s="27"/>
+      <c r="AM6" s="27"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3 E3:J3">
@@ -2193,8 +2219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2275,10 +2301,10 @@
         <v>46</v>
       </c>
       <c r="R1" s="21" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="S1" s="21" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="T1" s="22" t="s">
         <v>61</v>
@@ -2292,31 +2318,31 @@
         <v>21</v>
       </c>
       <c r="B2" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="H2" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="27" t="s">
-        <v>110</v>
-      </c>
-      <c r="D2" s="35" t="s">
-        <v>106</v>
-      </c>
-      <c r="E2" s="37" t="s">
-        <v>107</v>
-      </c>
-      <c r="F2" s="37" t="s">
+      <c r="I2" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="J2" s="36" t="s">
         <v>112</v>
-      </c>
-      <c r="H2" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="I2" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="J2" s="36" t="s">
-        <v>115</v>
       </c>
       <c r="K2" s="37" t="s">
         <v>66</v>
@@ -2328,13 +2354,13 @@
         <v>73</v>
       </c>
       <c r="N2" s="36" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="O2" s="35" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="P2" s="27" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q2" s="38"/>
       <c r="R2" s="39"/>
@@ -2347,31 +2373,31 @@
         <v>21</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F3" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="I3" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="J3" s="36" t="s">
         <v>112</v>
-      </c>
-      <c r="H3" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="I3" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="J3" s="36" t="s">
-        <v>115</v>
       </c>
       <c r="K3" s="37" t="s">
         <v>66</v>
@@ -2383,13 +2409,13 @@
         <v>73</v>
       </c>
       <c r="N3" s="36" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="O3" s="35" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="P3" s="27" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="Q3" s="38"/>
       <c r="R3" s="39"/>
@@ -2402,31 +2428,31 @@
         <v>21</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F4" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="G4" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="H4" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="I4" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G4" s="37" t="s">
+      <c r="J4" s="36" t="s">
         <v>112</v>
-      </c>
-      <c r="H4" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="I4" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="J4" s="36" t="s">
-        <v>115</v>
       </c>
       <c r="K4" s="37" t="s">
         <v>66</v>
@@ -2438,13 +2464,13 @@
         <v>73</v>
       </c>
       <c r="N4" s="36" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="O4" s="35" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="P4" s="27" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="Q4" s="38"/>
       <c r="R4" s="39"/>
@@ -2454,34 +2480,34 @@
     </row>
     <row r="5" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F5" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="G5" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="H5" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="I5" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G5" s="37" t="s">
+      <c r="J5" s="36" t="s">
         <v>112</v>
-      </c>
-      <c r="H5" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="I5" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="J5" s="36" t="s">
-        <v>115</v>
       </c>
       <c r="K5" s="37" t="s">
         <v>66</v>
@@ -2493,13 +2519,13 @@
         <v>73</v>
       </c>
       <c r="N5" s="36" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="O5" s="35" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="P5" s="27" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="Q5" s="38"/>
       <c r="R5" s="39"/>
@@ -2509,34 +2535,34 @@
     </row>
     <row r="6" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F6" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="G6" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="I6" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="J6" s="36" t="s">
         <v>112</v>
-      </c>
-      <c r="H6" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="I6" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="J6" s="36" t="s">
-        <v>115</v>
       </c>
       <c r="K6" s="37" t="s">
         <v>66</v>
@@ -2548,13 +2574,13 @@
         <v>73</v>
       </c>
       <c r="N6" s="36" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="O6" s="35" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="P6" s="27" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Q6" s="38"/>
       <c r="R6" s="39"/>

</xml_diff>